<commit_message>
Added data for new work package
</commit_message>
<xml_diff>
--- a/data/facilities_management/RM3830 assessed value services and UoM v6.xlsx
+++ b/data/facilities_management/RM3830 assessed value services and UoM v6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damola.salako/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manfrommons/Documents/GitHub/crown-marketplace/data/facilities_management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5265C1-8FA4-F245-960D-C958C39AC83B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39B6E86-FDB5-F447-ABEC-6F9C830D13E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36860" yWindow="460" windowWidth="27240" windowHeight="16040" xr2:uid="{E8FACC5C-8F0B-A349-8652-AD772759F213}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21600" windowHeight="37940" xr2:uid="{E8FACC5C-8F0B-A349-8652-AD772759F213}"/>
   </bookViews>
   <sheets>
     <sheet name="services and UoM" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="298">
   <si>
     <t>Work Package</t>
   </si>
@@ -910,6 +910,15 @@
   </si>
   <si>
     <t>B.1</t>
+  </si>
+  <si>
+    <t>Work Package O - Management of Billable Works</t>
+  </si>
+  <si>
+    <t>O.1</t>
+  </si>
+  <si>
+    <t>Management of Billable Works</t>
   </si>
 </sst>
 </file>
@@ -942,7 +951,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1163,11 +1172,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1259,6 +1277,10 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1573,9 +1595,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7676F3A0-BD13-1848-959C-0C3D52C42D72}">
-  <dimension ref="A1:G155"/>
+  <dimension ref="A1:G156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B89" workbookViewId="0">
+      <selection activeCell="D147" sqref="D147"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4458,65 +4482,63 @@
         <v>1.4539402376910019E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="16" t="s">
+    <row r="146" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A146" s="31" t="s">
         <v>281</v>
       </c>
-      <c r="B146" s="17" t="s">
+      <c r="B146" s="33" t="s">
         <v>282</v>
       </c>
-      <c r="C146" s="17"/>
-      <c r="D146" s="18" t="s">
+      <c r="C146" s="33"/>
+      <c r="D146" s="33" t="s">
         <v>283</v>
       </c>
-      <c r="E146" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F146" s="19">
+      <c r="E146" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F146" s="33">
         <v>2.9853806818889703E-2</v>
       </c>
-      <c r="G146" s="20">
+      <c r="G146" s="34">
         <v>2.9853806818889703E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="149" spans="1:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="A149" s="26" t="s">
+    <row r="147" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="16" t="s">
+        <v>295</v>
+      </c>
+      <c r="B147" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="C147" s="17"/>
+      <c r="D147" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="E147" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F147" s="19"/>
+      <c r="G147" s="20"/>
+    </row>
+    <row r="149" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="150" spans="1:7" ht="15" x14ac:dyDescent="0.15">
+      <c r="A150" s="26" t="s">
         <v>293</v>
       </c>
-      <c r="B149" s="27" t="s">
+      <c r="B150" s="27" t="s">
         <v>294</v>
       </c>
-      <c r="C149" s="27"/>
-      <c r="D149" s="28" t="s">
+      <c r="C150" s="27"/>
+      <c r="D150" s="28" t="s">
         <v>293</v>
       </c>
-      <c r="E149" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="F149" s="29">
+      <c r="E150" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F150" s="29">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="G149" s="30"/>
-    </row>
-    <row r="150" spans="1:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="A150" s="11" t="s">
-        <v>284</v>
-      </c>
-      <c r="B150" s="12"/>
-      <c r="C150" s="12"/>
-      <c r="D150" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="E150" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F150" s="22">
-        <v>0.10090441334513844</v>
-      </c>
-      <c r="G150" s="23">
-        <v>0.10090441334513844</v>
-      </c>
+      <c r="G150" s="30"/>
     </row>
     <row r="151" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A151" s="11" t="s">
@@ -4525,16 +4547,16 @@
       <c r="B151" s="12"/>
       <c r="C151" s="12"/>
       <c r="D151" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E151" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F151" s="22">
-        <v>4.2000000000000003E-2</v>
+        <v>0.10090441334513844</v>
       </c>
       <c r="G151" s="23">
-        <v>4.9824514991181672E-2</v>
+        <v>0.10090441334513844</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="15" x14ac:dyDescent="0.15">
@@ -4544,72 +4566,91 @@
       <c r="B152" s="12"/>
       <c r="C152" s="12"/>
       <c r="D152" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E152" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F152" s="22">
-        <v>3.1E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="G152" s="23">
-        <v>5.427986509620053E-2</v>
+        <v>4.9824514991181672E-2</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A153" s="11" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B153" s="12"/>
       <c r="C153" s="12"/>
       <c r="D153" s="13" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E153" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F153" s="22">
-        <v>0.18811284090909089</v>
+        <v>3.1E-2</v>
       </c>
       <c r="G153" s="23">
-        <v>0.18811284090909089</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" ht="30" x14ac:dyDescent="0.15">
+        <v>5.427986509620053E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A154" s="11" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B154" s="12"/>
       <c r="C154" s="12"/>
       <c r="D154" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="E154" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F154" s="22">
+        <v>0.18811284090909089</v>
+      </c>
+      <c r="G154" s="23">
+        <v>0.18811284090909089</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" ht="30" x14ac:dyDescent="0.15">
+      <c r="A155" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="B155" s="12"/>
+      <c r="C155" s="12"/>
+      <c r="D155" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="E154" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F154" s="14">
+      <c r="E155" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F155" s="14">
         <v>26.209131601009094</v>
       </c>
-      <c r="G154" s="15">
+      <c r="G155" s="15">
         <v>26.209131601009094</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="16" t="s">
+    <row r="156" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="B155" s="17"/>
-      <c r="C155" s="17"/>
-      <c r="D155" s="18" t="s">
+      <c r="B156" s="17"/>
+      <c r="C156" s="17"/>
+      <c r="D156" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="E155" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F155" s="24">
+      <c r="E156" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F156" s="24">
         <v>0.10383703703703703</v>
       </c>
-      <c r="G155" s="25">
+      <c r="G156" s="25">
         <v>0.10383703703703703</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Feature/fm 488 detailed search results fc (#1524)
* Added data for new work package

* Changes in the Schema file

* New layout for FC procurements
New Layout helper to aid conditional rendering

* Rubocop
</commit_message>
<xml_diff>
--- a/data/facilities_management/RM3830 assessed value services and UoM v6.xlsx
+++ b/data/facilities_management/RM3830 assessed value services and UoM v6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damola.salako/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manfrommons/Documents/GitHub/crown-marketplace/data/facilities_management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5265C1-8FA4-F245-960D-C958C39AC83B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39B6E86-FDB5-F447-ABEC-6F9C830D13E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36860" yWindow="460" windowWidth="27240" windowHeight="16040" xr2:uid="{E8FACC5C-8F0B-A349-8652-AD772759F213}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21600" windowHeight="37940" xr2:uid="{E8FACC5C-8F0B-A349-8652-AD772759F213}"/>
   </bookViews>
   <sheets>
     <sheet name="services and UoM" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="298">
   <si>
     <t>Work Package</t>
   </si>
@@ -910,6 +910,15 @@
   </si>
   <si>
     <t>B.1</t>
+  </si>
+  <si>
+    <t>Work Package O - Management of Billable Works</t>
+  </si>
+  <si>
+    <t>O.1</t>
+  </si>
+  <si>
+    <t>Management of Billable Works</t>
   </si>
 </sst>
 </file>
@@ -942,7 +951,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1163,11 +1172,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1259,6 +1277,10 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1573,9 +1595,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7676F3A0-BD13-1848-959C-0C3D52C42D72}">
-  <dimension ref="A1:G155"/>
+  <dimension ref="A1:G156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B89" workbookViewId="0">
+      <selection activeCell="D147" sqref="D147"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4458,65 +4482,63 @@
         <v>1.4539402376910019E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="16" t="s">
+    <row r="146" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A146" s="31" t="s">
         <v>281</v>
       </c>
-      <c r="B146" s="17" t="s">
+      <c r="B146" s="33" t="s">
         <v>282</v>
       </c>
-      <c r="C146" s="17"/>
-      <c r="D146" s="18" t="s">
+      <c r="C146" s="33"/>
+      <c r="D146" s="33" t="s">
         <v>283</v>
       </c>
-      <c r="E146" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F146" s="19">
+      <c r="E146" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F146" s="33">
         <v>2.9853806818889703E-2</v>
       </c>
-      <c r="G146" s="20">
+      <c r="G146" s="34">
         <v>2.9853806818889703E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="149" spans="1:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="A149" s="26" t="s">
+    <row r="147" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="16" t="s">
+        <v>295</v>
+      </c>
+      <c r="B147" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="C147" s="17"/>
+      <c r="D147" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="E147" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F147" s="19"/>
+      <c r="G147" s="20"/>
+    </row>
+    <row r="149" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="150" spans="1:7" ht="15" x14ac:dyDescent="0.15">
+      <c r="A150" s="26" t="s">
         <v>293</v>
       </c>
-      <c r="B149" s="27" t="s">
+      <c r="B150" s="27" t="s">
         <v>294</v>
       </c>
-      <c r="C149" s="27"/>
-      <c r="D149" s="28" t="s">
+      <c r="C150" s="27"/>
+      <c r="D150" s="28" t="s">
         <v>293</v>
       </c>
-      <c r="E149" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="F149" s="29">
+      <c r="E150" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F150" s="29">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="G149" s="30"/>
-    </row>
-    <row r="150" spans="1:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="A150" s="11" t="s">
-        <v>284</v>
-      </c>
-      <c r="B150" s="12"/>
-      <c r="C150" s="12"/>
-      <c r="D150" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="E150" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F150" s="22">
-        <v>0.10090441334513844</v>
-      </c>
-      <c r="G150" s="23">
-        <v>0.10090441334513844</v>
-      </c>
+      <c r="G150" s="30"/>
     </row>
     <row r="151" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A151" s="11" t="s">
@@ -4525,16 +4547,16 @@
       <c r="B151" s="12"/>
       <c r="C151" s="12"/>
       <c r="D151" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E151" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F151" s="22">
-        <v>4.2000000000000003E-2</v>
+        <v>0.10090441334513844</v>
       </c>
       <c r="G151" s="23">
-        <v>4.9824514991181672E-2</v>
+        <v>0.10090441334513844</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="15" x14ac:dyDescent="0.15">
@@ -4544,72 +4566,91 @@
       <c r="B152" s="12"/>
       <c r="C152" s="12"/>
       <c r="D152" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E152" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F152" s="22">
-        <v>3.1E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="G152" s="23">
-        <v>5.427986509620053E-2</v>
+        <v>4.9824514991181672E-2</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A153" s="11" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B153" s="12"/>
       <c r="C153" s="12"/>
       <c r="D153" s="13" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E153" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F153" s="22">
-        <v>0.18811284090909089</v>
+        <v>3.1E-2</v>
       </c>
       <c r="G153" s="23">
-        <v>0.18811284090909089</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" ht="30" x14ac:dyDescent="0.15">
+        <v>5.427986509620053E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A154" s="11" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B154" s="12"/>
       <c r="C154" s="12"/>
       <c r="D154" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="E154" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F154" s="22">
+        <v>0.18811284090909089</v>
+      </c>
+      <c r="G154" s="23">
+        <v>0.18811284090909089</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" ht="30" x14ac:dyDescent="0.15">
+      <c r="A155" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="B155" s="12"/>
+      <c r="C155" s="12"/>
+      <c r="D155" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="E154" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F154" s="14">
+      <c r="E155" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F155" s="14">
         <v>26.209131601009094</v>
       </c>
-      <c r="G154" s="15">
+      <c r="G155" s="15">
         <v>26.209131601009094</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="16" t="s">
+    <row r="156" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="B155" s="17"/>
-      <c r="C155" s="17"/>
-      <c r="D155" s="18" t="s">
+      <c r="B156" s="17"/>
+      <c r="C156" s="17"/>
+      <c r="D156" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="E155" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F155" s="24">
+      <c r="E156" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F156" s="24">
         <v>0.10383703703703703</v>
       </c>
-      <c r="G155" s="25">
+      <c r="G156" s="25">
         <v>0.10383703703703703</v>
       </c>
     </row>

</xml_diff>